<commit_message>
Commit to merge 2
</commit_message>
<xml_diff>
--- a/Scrum/Backlogs/Backlog Week 5.xlsx
+++ b/Scrum/Backlogs/Backlog Week 5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johannes\template\Scrum\Backlogs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D039F48C-0439-47E4-8D75-3F89C686B099}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31095607-DBAD-4C31-B9D8-846ECFDC4CE0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>I am a user and I am interested in knowing how much CO2 I save with one vegetarian meal</t>
   </si>
   <si>
-    <t>Create an implementation of the vegetarian meal process</t>
-  </si>
-  <si>
     <t>Implement a Restful server with a connection to a database via hibernate</t>
   </si>
   <si>
@@ -127,10 +124,13 @@
     <t>Connecting the database to the server via hibernate</t>
   </si>
   <si>
-    <t>Look into the RestAPI to create a client</t>
+    <t>I am a developer - I need this in order to be able to communicate with the server</t>
   </si>
   <si>
-    <t>I am a developer - I need this in order to be able to communicate with the server</t>
+    <t>Look into the RestAPI to create a client, create an implementation of the vegetarian meal process, create an account screen</t>
+  </si>
+  <si>
+    <t>Create an implementation of the vegetarian meal process and the writing to file class</t>
   </si>
 </sst>
 </file>
@@ -646,7 +646,7 @@
   <dimension ref="A1:Z1011"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1058,10 +1058,10 @@
     <row r="14" spans="1:26" ht="39.6">
       <c r="A14" s="1"/>
       <c r="B14" s="23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D14" s="24" t="s">
         <v>23</v>
@@ -1095,13 +1095,13 @@
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
     </row>
-    <row r="15" spans="1:26" ht="52.8">
+    <row r="15" spans="1:26" ht="66">
       <c r="A15" s="1"/>
       <c r="B15" s="23" t="s">
         <v>27</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D15" s="24" t="s">
         <v>17</v>
@@ -1141,7 +1141,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>20</v>
@@ -1175,10 +1175,10 @@
       <c r="Y16" s="1"/>
       <c r="Z16" s="1"/>
     </row>
-    <row r="17" spans="1:26" ht="39.6">
+    <row r="17" spans="1:26" ht="92.4">
       <c r="A17" s="1"/>
       <c r="B17" s="23" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C17" s="23" t="s">
         <v>35</v>
@@ -1221,7 +1221,7 @@
         <v>27</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>18</v>
@@ -1258,10 +1258,10 @@
     <row r="19" spans="1:26" ht="39.6">
       <c r="A19" s="1"/>
       <c r="B19" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>21</v>

</xml_diff>